<commit_message>
feat: More descriptive error messages
- I've improved the error messages when trying to download the video to make them more descriptive, and therefore give more feedback to the user.
</commit_message>
<xml_diff>
--- a/src/settings_files/languages.xlsx
+++ b/src/settings_files/languages.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raulc\Desktop\Dev\Apps\Apps_Python\Proyectos\EasyViewer\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raulc\Desktop\Dev\Apps\Apps_Python\Proyectos\EasyViewer\src\settings_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F7A006-EFB6-4DCA-948D-9F14C9C62D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D50B52C-75C8-4445-991D-EE6612E92CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
   <si>
     <t>Español</t>
   </si>
@@ -162,14 +162,50 @@
 No update is required at this time.</t>
   </si>
   <si>
-    <t>Algo ha ido mal. 
-Por favor, inténtalo de nuevo más tarde. 
-Si el problema persiste, contacta conmigo a través de mis redes sociales</t>
-  </si>
-  <si>
-    <t>Something has gone wrong. 
-Please try again later. 
-If the problem persists, contact me through my social networks</t>
+    <t xml:space="preserve"> Ocurrió un error al descargar el video. Inténtalo nuevamente más tarde.</t>
+  </si>
+  <si>
+    <t>There was an error downloading the video. Try again later.</t>
+  </si>
+  <si>
+    <t>This video is unavailable.</t>
+  </si>
+  <si>
+    <t>This video is blocked in your region.</t>
+  </si>
+  <si>
+    <t>This video is private.</t>
+  </si>
+  <si>
+    <t>This video is only available to members.</t>
+  </si>
+  <si>
+    <t>Este video no está disponible.</t>
+  </si>
+  <si>
+    <t>Este video está bloqueado en tu región.</t>
+  </si>
+  <si>
+    <t>Este video es privado.</t>
+  </si>
+  <si>
+    <t>Este video solo está disponible para miembros.</t>
+  </si>
+  <si>
+    <t>This video is age restricted. 
+You can't download it.</t>
+  </si>
+  <si>
+    <t>Este video tiene restricción de edad. 
+No puedes descargarlo.</t>
+  </si>
+  <si>
+    <t>La transmisión en directo todavía esta vigente. 
+Vuelve a intentarlo cuando haya finalizado</t>
+  </si>
+  <si>
+    <t>The live stream is still live. 
+Please try again when it has finished</t>
   </si>
 </sst>
 </file>
@@ -546,16 +582,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="70.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="54.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="56.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -742,7 +778,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>43</v>
       </c>
@@ -750,13 +786,64 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B31" s="5" t="s">
         <v>47</v>
       </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: Improved error message during download
- Relocated error handling from 'interact_api_pytube.py' to 'validations.py'.
- Enhanced the error message to include guidance for users: 'If the error persists, please contact me.'
</commit_message>
<xml_diff>
--- a/src/settings_files/languages.xlsx
+++ b/src/settings_files/languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raulc\Desktop\Dev\Apps\Apps_Python\Proyectos\EasyViewer\src\settings_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D50B52C-75C8-4445-991D-EE6612E92CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B001496-6487-4285-99A1-6C2BBED74685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -162,12 +162,6 @@
 No update is required at this time.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Ocurrió un error al descargar el video. Inténtalo nuevamente más tarde.</t>
-  </si>
-  <si>
-    <t>There was an error downloading the video. Try again later.</t>
-  </si>
-  <si>
     <t>This video is unavailable.</t>
   </si>
   <si>
@@ -206,6 +200,16 @@
   <si>
     <t>The live stream is still live. 
 Please try again when it has finished</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ocurrió un error al descargar el video. 
+Inténtalo nuevamente más tarde.
+Si el error persiste, ponte en contacto conmigo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> An error occurred while downloading the video. 
+Please try again later.
+If the error persists, please contact me.</t>
   </si>
 </sst>
 </file>
@@ -584,8 +588,8 @@
   </sheetPr>
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,58 +792,58 @@
     </row>
     <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>47</v>
+    </row>
+    <row r="31" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat: Introduced 'What's New' dialog box
- Now, the app displays 'What's New' information using text files, enabling easier updates for future changes.
- Language-specific 'What's New' content is sourced from 'whats_new_es.txt' (for Spanish) and 'whats_new_en.txt' (for English).
</commit_message>
<xml_diff>
--- a/src/settings_files/languages.xlsx
+++ b/src/settings_files/languages.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raulc\Desktop\Dev\Apps\Apps_Python\Proyectos\EasyViewer\src\settings_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B001496-6487-4285-99A1-6C2BBED74685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35ECF6E-19A5-4936-8BFA-075274A2C44D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t>Español</t>
   </si>
@@ -210,6 +210,12 @@
     <t xml:space="preserve"> An error occurred while downloading the video. 
 Please try again later.
 If the error persists, please contact me.</t>
+  </si>
+  <si>
+    <t>¿Que hay de nuevo?</t>
+  </si>
+  <si>
+    <t>What's new?</t>
   </si>
 </sst>
 </file>
@@ -588,8 +594,8 @@
   </sheetPr>
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,7 +853,12 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="5"/>
+      <c r="A32" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add disclaimer dialog for YouTube T&C violations
- Added a dialog to disclaim responsibility for YouTube T&C violations when downloading videos.
- Note: There is a bug preventing the dialog from displaying properly.
</commit_message>
<xml_diff>
--- a/src/settings_files/languages.xlsx
+++ b/src/settings_files/languages.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raulc\Desktop\Dev\Apps\Apps_Python\Proyectos\EasyViewer\src\settings_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raulc\Desktop\Dev\Proyectos\Python\EasyViewer\src\settings_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35ECF6E-19A5-4936-8BFA-075274A2C44D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF7A89D-C147-4924-895E-2FFD5448A271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
   <si>
     <t>Español</t>
   </si>
@@ -216,6 +216,20 @@
   </si>
   <si>
     <t>What's new?</t>
+  </si>
+  <si>
+    <t>Al utilizar esta aplicación para descargar videos de YouTube, usted acepta que no nos hacemos responsables por cualquier incumplimiento de los términos y condiciones de YouTube. 
+Es importante que revise y cumpla con las políticas de YouTube antes usar comercialmente cualquier contenido descargado a través de la app.</t>
+  </si>
+  <si>
+    <t>By using this app to download videos from YouTube, you agree that we're not responsible for any failure to comply with YouTube's terms and conditions. 
+It's important that you review and comply with YouTube's policies before commercially using any content downloaded through the app.</t>
+  </si>
+  <si>
+    <t>Aviso de responsabilidad</t>
+  </si>
+  <si>
+    <t>Liability notice</t>
   </si>
 </sst>
 </file>
@@ -592,10 +606,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,6 +874,22 @@
         <v>61</v>
       </c>
     </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>